<commit_message>
final approval of act recognition
</commit_message>
<xml_diff>
--- a/input documents/CRS/Review/PO_SAG_CRS_Act_Recog_Review.xlsx
+++ b/input documents/CRS/Review/PO_SAG_CRS_Act_Recog_Review.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Graduation Project\github_repos\ML_SWProcess_Documents\input documents\CRS\Review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1165D88-3D1E-4107-944F-70E502C1994D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB81BC1-9318-498B-87AB-84A620B92241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
   <si>
     <t>DocType_REV_ID</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>change Document Status to last Document History</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>CRS_REVIEW_001</t>
@@ -641,22 +638,22 @@
   <dimension ref="A1:H98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" customWidth="1"/>
-    <col min="5" max="5" width="35.6640625" customWidth="1"/>
-    <col min="6" max="6" width="62.44140625" customWidth="1"/>
-    <col min="7" max="7" width="48.33203125" customWidth="1"/>
-    <col min="8" max="8" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="32.28515625" customWidth="1"/>
+    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="6" max="6" width="62.42578125" customWidth="1"/>
+    <col min="7" max="7" width="48.28515625" customWidth="1"/>
+    <col min="8" max="8" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -682,259 +679,259 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="3">
         <v>44877</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" s="3">
         <v>44877</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="3">
         <v>44877</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="3">
         <v>44877</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
         <v>44877</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
-        <v>33</v>
       </c>
       <c r="B7" s="3">
         <v>44880</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="H7" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B8" s="3">
         <v>44880</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="3">
         <v>44880</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F9" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="G9" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="3">
         <v>44880</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="G10" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="3">
         <v>44880</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="G11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="3"/>
       <c r="C12" s="2"/>
@@ -944,7 +941,7 @@
       <c r="G12" s="2"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
       <c r="B13" s="3"/>
       <c r="C13" s="2"/>
@@ -954,91 +951,91 @@
       <c r="G13" s="2"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A2:H7">

</xml_diff>